<commit_message>
Redesigned POS3P3 supply with new controller for 5 amps
</commit_message>
<xml_diff>
--- a/hdw/Logic_Board/LED_Display_Controller/LED_Display_Controller_bom_A.xlsx
+++ b/hdw/Logic_Board/LED_Display_Controller/LED_Display_Controller_bom_A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\Electronic_Display\hdw\Logic_Board\LED_Display_Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9E7C133B-4024-47B6-956A-E74A9AE48640}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{16BBAC70-DEB9-44BB-8883-5C07AEE1DE79}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10020"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="265">
   <si>
     <t>References</t>
   </si>
@@ -34,7 +34,7 @@
     <t>Digi-Key PN</t>
   </si>
   <si>
-    <t>C201 C204 C403 C405 C501 C502 C601 C602 C603 C611 C612 C613 C620 C621 C622 C902 C905 C1001 C1003 C1101 C1102 C1103 C1104 C1105 C1107 C1108 C1111 C1201 C1202 C1203 C1204 C1205 C1206 C1207 C1301 C1302 C1303 C1304 C1401 C1402 C1403 C1404 C1405 C1602 C1603 C1604 C1605 C1607 C1608 C1609 C1701 C1704 C1801 C1901 C2001 C2101 C2201 C2301 C2401 C2501 C2601 C2602 C2701 C2702 C2801 C2802</t>
+    <t>C201 C204 C305 C307 C403 C405 C501 C502 C601 C602 C603 C611 C612 C613 C620 C621 C622 C902 C905 C1001 C1003 C1101 C1102 C1103 C1104 C1105 C1107 C1108 C1111 C1201 C1202 C1203 C1204 C1205 C1206 C1207 C1301 C1302 C1303 C1304 C1401 C1402 C1403 C1404 C1405 C1602 C1603 C1604 C1605 C1607 C1608 C1609 C1701 C1704 C1801 C1901 C2001 C2101 C2201 C2301 C2401 C2501 C2601 C2602 C2701 C2702 C2801 C2802</t>
   </si>
   <si>
     <t>0.1uF</t>
@@ -43,15 +43,6 @@
     <t>311-1344-1-ND</t>
   </si>
   <si>
-    <t>C305</t>
-  </si>
-  <si>
-    <t>0.22uF</t>
-  </si>
-  <si>
-    <t>490-5402-1-ND</t>
-  </si>
-  <si>
     <t>C1002</t>
   </si>
   <si>
@@ -61,16 +52,7 @@
     <t>565-4707-1-ND</t>
   </si>
   <si>
-    <t>C301 C302</t>
-  </si>
-  <si>
-    <t>100pF</t>
-  </si>
-  <si>
-    <t>311-1069-1-ND</t>
-  </si>
-  <si>
-    <t>C309 C604 C901 C1606</t>
+    <t>C604 C901 C1606</t>
   </si>
   <si>
     <t>100uF</t>
@@ -85,7 +67,7 @@
     <t>718-1102-1-ND</t>
   </si>
   <si>
-    <t>C202 C605 C606 C607 C614 C615 C616 C623 C624 C625 C903 C1702 C1705 C1802 C1902 C2002 C2102 C2202 C2302 C2402 C2502 C2603 C2604 C2703 C2704 C2803</t>
+    <t>C202 C304 C605 C606 C607 C614 C615 C616 C623 C624 C625 C903 C1702 C1705 C1802 C1902 C2002 C2102 C2202 C2302 C2402 C2502 C2603 C2604 C2703 C2704 C2803</t>
   </si>
   <si>
     <t>10nF</t>
@@ -103,10 +85,13 @@
     <t>478-8236-1-ND</t>
   </si>
   <si>
-    <t>C308</t>
-  </si>
-  <si>
-    <t>587-3401-1-ND</t>
+    <t>C308 C310</t>
+  </si>
+  <si>
+    <t>15pF</t>
+  </si>
+  <si>
+    <t>478-10289-1-ND</t>
   </si>
   <si>
     <t>C203 C608 C609 C610 C617 C618 C619 C626 C627 C628 C904 C1703 C1706 C1803 C1903 C2003 C2103 C2203 C2303 C2403 C2503 C2605 C2606 C2705 C2706 C2804</t>
@@ -118,76 +103,76 @@
     <t>1276-1018-1-ND</t>
   </si>
   <si>
+    <t>C309 C401</t>
+  </si>
+  <si>
+    <t>2.2uF</t>
+  </si>
+  <si>
+    <t>445-5691-1-ND</t>
+  </si>
+  <si>
+    <t>C301 C302 C303 C402 C406 C407</t>
+  </si>
+  <si>
+    <t>22uF</t>
+  </si>
+  <si>
+    <t>445-1453-1-ND</t>
+  </si>
+  <si>
+    <t>C1501 C1502 C1503 C1504 C1505</t>
+  </si>
+  <si>
+    <t>330pF</t>
+  </si>
+  <si>
+    <t>399-6880-1-ND</t>
+  </si>
+  <si>
+    <t>C404</t>
+  </si>
+  <si>
+    <t>33pF</t>
+  </si>
+  <si>
+    <t>399-1055-1-ND</t>
+  </si>
+  <si>
+    <t>C1106</t>
+  </si>
+  <si>
+    <t>4.7uF</t>
+  </si>
+  <si>
+    <t>1276-2972-1-ND</t>
+  </si>
+  <si>
+    <t>C1109 C1110</t>
+  </si>
+  <si>
+    <t>47pF</t>
+  </si>
+  <si>
+    <t>478-1171-1-ND</t>
+  </si>
+  <si>
+    <t>C311 C312</t>
+  </si>
+  <si>
+    <t>47uF</t>
+  </si>
+  <si>
+    <t>490-4844-1-ND</t>
+  </si>
+  <si>
     <t>C306</t>
   </si>
   <si>
-    <t>1uF</t>
-  </si>
-  <si>
-    <t>587-3247-1-ND</t>
-  </si>
-  <si>
-    <t>C401</t>
-  </si>
-  <si>
-    <t>2.2uF</t>
-  </si>
-  <si>
-    <t>445-5691-1-ND</t>
-  </si>
-  <si>
-    <t>C307</t>
-  </si>
-  <si>
-    <t>22pF</t>
-  </si>
-  <si>
-    <t>478-1167-1-ND</t>
-  </si>
-  <si>
-    <t>C303 C402 C406 C407</t>
-  </si>
-  <si>
-    <t>22uF</t>
-  </si>
-  <si>
-    <t>445-1453-1-ND</t>
-  </si>
-  <si>
-    <t>C304 C1501 C1502 C1503 C1504 C1505</t>
-  </si>
-  <si>
-    <t>330pF</t>
-  </si>
-  <si>
-    <t>399-6880-1-ND</t>
-  </si>
-  <si>
-    <t>C404</t>
-  </si>
-  <si>
-    <t>33pF</t>
-  </si>
-  <si>
-    <t>399-1055-1-ND</t>
-  </si>
-  <si>
-    <t>C1106</t>
-  </si>
-  <si>
-    <t>4.7uF</t>
-  </si>
-  <si>
-    <t>1276-2972-1-ND</t>
-  </si>
-  <si>
-    <t>C1109 C1110</t>
-  </si>
-  <si>
-    <t>47pF</t>
-  </si>
-  <si>
-    <t>478-1171-1-ND</t>
+    <t>62pF</t>
+  </si>
+  <si>
+    <t>1276-2320-1-ND</t>
   </si>
   <si>
     <t>D202</t>
@@ -415,10 +400,10 @@
     <t>L301</t>
   </si>
   <si>
-    <t>2.2uH</t>
-  </si>
-  <si>
-    <t>541-1236-1-ND</t>
+    <t>0.47uH</t>
+  </si>
+  <si>
+    <t>541-1231-1-ND</t>
   </si>
   <si>
     <t>L401</t>
@@ -484,7 +469,7 @@
     <t>311-0.0GRCT-ND</t>
   </si>
   <si>
-    <t>R205 R206 R501 R908</t>
+    <t>R205 R206 R304 R501 R908</t>
   </si>
   <si>
     <t>YAG3351CT-ND</t>
@@ -496,7 +481,7 @@
     <t>A106047CT-ND</t>
   </si>
   <si>
-    <t>R204 R405</t>
+    <t>R204 R302 R307 R405</t>
   </si>
   <si>
     <t>100k</t>
@@ -505,16 +490,7 @@
     <t>A106046CT-ND</t>
   </si>
   <si>
-    <t>R303 R305</t>
-  </si>
-  <si>
-    <t>105k</t>
-  </si>
-  <si>
-    <t>311-105KHRCT-ND</t>
-  </si>
-  <si>
-    <t>R207 R301 R302 R304 R401 R402 R403 R404 R502 R504 R902 R903 R904 R905 R907 R1003 R1004 R1005 R1006 R1101 R1105 R1201 R1202 R1205 R1206 R1209 R1210 R1213 R1401 R1402 R1405 R1406 R1407 R1408 R1501 R1502 R1503 R1504 R1505 R1506 R1507 R1508 R1509 R1605 R1606 R1607 R1608 R1609 R1610 R1806 R1807 R1808 R1809 R1810 R1811 R1906 R1907 R1908 R1909 R1910 R1911 R2006 R2007 R2008 R2009 R2010 R2011 R2106 R2107 R2108 R2109 R2110 R2111 R2206 R2207 R2208 R2209 R2210 R2211 R2306 R2307 R2308 R2309 R2310 R2311 R2406 R2407 R2408 R2409 R2410 R2411 R2506 R2507 R2508 R2509 R2510 R2511 R2613 R2614 R2615 R2616 R2617 R2618 R2619 R2620 R2621 R2622 R2623 R2624 R2625 R2626 R2627 R2628 R2629 R2630 R2631 R2632 R2633 R2634 R2635 R2636 R2637 R2638 R2639 R2640 R2641 R2642 R2713 R2714 R2715 R2716 R2717 R2718 R2719 R2720 R2721 R2722 R2723 R2724 R2725 R2726 R2727 R2728 R2729 R2730 R2731 R2732 R2733 R2734 R2735 R2736 R2737 R2738 R2739 R2740 R2741 R2742 R2803 R2804 R2813 R2814 R2815 R2816 R2817 R2818 R2819 R2820 R2821 R2822 R2823 R2824 R2825 R2826 R2827 R2828 R2829</t>
+    <t>R207 R301 R401 R402 R403 R404 R502 R504 R902 R903 R904 R905 R907 R1003 R1004 R1005 R1006 R1101 R1105 R1201 R1202 R1205 R1206 R1209 R1210 R1213 R1401 R1402 R1405 R1406 R1407 R1408 R1501 R1502 R1503 R1504 R1505 R1506 R1507 R1508 R1509 R1605 R1606 R1607 R1608 R1609 R1610 R1806 R1807 R1808 R1809 R1810 R1811 R1906 R1907 R1908 R1909 R1910 R1911 R2006 R2007 R2008 R2009 R2010 R2011 R2106 R2107 R2108 R2109 R2110 R2111 R2206 R2207 R2208 R2209 R2210 R2211 R2306 R2307 R2308 R2309 R2310 R2311 R2406 R2407 R2408 R2409 R2410 R2411 R2506 R2507 R2508 R2509 R2510 R2511 R2613 R2614 R2615 R2616 R2617 R2618 R2619 R2620 R2621 R2622 R2623 R2624 R2625 R2626 R2627 R2628 R2629 R2630 R2631 R2632 R2633 R2634 R2635 R2636 R2637 R2638 R2639 R2640 R2641 R2642 R2713 R2714 R2715 R2716 R2717 R2718 R2719 R2720 R2721 R2722 R2723 R2724 R2725 R2726 R2727 R2728 R2729 R2730 R2731 R2732 R2733 R2734 R2735 R2736 R2737 R2738 R2739 R2740 R2741 R2742 R2803 R2804 R2813 R2814 R2815 R2816 R2817 R2818 R2819 R2820 R2821 R2822 R2823 R2824 R2825 R2826 R2827 R2828 R2829</t>
   </si>
   <si>
     <t>10k</t>
@@ -523,6 +499,15 @@
     <t>RMCF0603FT10K0CT-ND</t>
   </si>
   <si>
+    <t>R306</t>
+  </si>
+  <si>
+    <t>13.3k</t>
+  </si>
+  <si>
+    <t>P13.3KHCT-ND</t>
+  </si>
+  <si>
     <t>R406</t>
   </si>
   <si>
@@ -532,15 +517,6 @@
     <t>P13.7KHCT-ND</t>
   </si>
   <si>
-    <t>R306</t>
-  </si>
-  <si>
-    <t>165k</t>
-  </si>
-  <si>
-    <t>RMCF0603FT165KCT-ND</t>
-  </si>
-  <si>
     <t>R506 R1106 R1109 R1203 R1204 R1207 R1208 R1211 R1212 R1214 R1301 R1302 R1303 R1304 R1403 R1404 R1510 R1603 R1604</t>
   </si>
   <si>
@@ -556,6 +532,15 @@
     <t>RMCF0603FT200RCT-ND</t>
   </si>
   <si>
+    <t>R303 R308</t>
+  </si>
+  <si>
+    <t>22.1k</t>
+  </si>
+  <si>
+    <t>P22.1KHCT-ND</t>
+  </si>
+  <si>
     <t>R203</t>
   </si>
   <si>
@@ -571,15 +556,6 @@
     <t>RMCF0603FT27R0CT-ND</t>
   </si>
   <si>
-    <t>R307</t>
-  </si>
-  <si>
-    <t>36.5k</t>
-  </si>
-  <si>
-    <t>311-36.5KHRCT-ND</t>
-  </si>
-  <si>
     <t>R1104</t>
   </si>
   <si>
@@ -625,6 +601,15 @@
     <t>RMCF0603FT6K04CT-ND</t>
   </si>
   <si>
+    <t>R305</t>
+  </si>
+  <si>
+    <t>63.4k</t>
+  </si>
+  <si>
+    <t>541-63.4KHCT-ND</t>
+  </si>
+  <si>
     <t>R1602</t>
   </si>
   <si>
@@ -760,13 +745,13 @@
     <t>LT6700CS6-1#TRMPBFCT-ND</t>
   </si>
   <si>
-    <t>LTC3603_UF</t>
+    <t>LTC3605A_UF</t>
   </si>
   <si>
     <t>U301</t>
   </si>
   <si>
-    <t>LTC3603EUF#PBF-ND</t>
+    <t>LTC3605AIUF#TRPBFCT-ND</t>
   </si>
   <si>
     <t>LTC3624DD</t>
@@ -1673,13 +1658,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="28.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.1796875" customWidth="1"/>
+    <col min="2" max="2" width="20.08984375" customWidth="1"/>
+    <col min="3" max="3" width="16.6328125" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -1695,7 +1686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="232" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1703,7 +1694,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -1731,7 +1722,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
@@ -1742,35 +1733,35 @@
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" s="1">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -1779,7 +1770,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -1787,13 +1778,13 @@
         <v>22</v>
       </c>
       <c r="C8" s="1">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1801,7 +1792,7 @@
         <v>25</v>
       </c>
       <c r="C9" s="1">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>26</v>
@@ -1812,252 +1803,250 @@
         <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C19" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C21" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C22" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="C23" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C24" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="C25" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="C27" s="1">
-        <v>7</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
@@ -2075,29 +2064,29 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
-      <c r="D29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
@@ -2109,16 +2098,14 @@
       <c r="C31" s="1">
         <v>1</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
@@ -2127,22 +2114,24 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="C33" s="1">
         <v>1</v>
       </c>
-      <c r="D33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
@@ -2151,24 +2140,22 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="C35" s="1">
         <v>1</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="D35" s="1"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
@@ -2177,10 +2164,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
@@ -2189,10 +2176,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="C38" s="1">
         <v>1</v>
@@ -2201,10 +2188,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="C39" s="1">
         <v>1</v>
@@ -2213,15 +2200,17 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C40" s="1">
-        <v>1</v>
-      </c>
-      <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
@@ -2233,20 +2222,22 @@
       <c r="C41" s="1">
         <v>1</v>
       </c>
-      <c r="D41" s="1"/>
+      <c r="D41" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C42" s="1">
-        <v>1</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
@@ -2260,49 +2251,47 @@
         <v>1</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="C44" s="1">
         <v>1</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="C45" s="1">
         <v>1</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>116</v>
-      </c>
+      <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="C46" s="1">
-        <v>1</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
@@ -2319,10 +2308,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="C48" s="1">
         <v>1</v>
@@ -2341,140 +2330,142 @@
       <c r="C49" s="1">
         <v>1</v>
       </c>
-      <c r="D49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C50" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C51" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C52" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>140</v>
       </c>
       <c r="C53" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C54" s="1">
-        <v>12</v>
-      </c>
-      <c r="D54" s="1" t="s">
+    </row>
+    <row r="55" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
+      <c r="C55" s="1">
+        <v>2</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C55" s="1">
-        <v>1</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C56" s="1">
-        <v>1</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B57" s="1">
+        <v>10</v>
+      </c>
+      <c r="C57" s="1">
+        <v>5</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C57" s="1">
-        <v>2</v>
-      </c>
-      <c r="D57" s="1" t="s">
+    </row>
+    <row r="58" spans="1:4" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" s="1" t="s">
+      <c r="B58" s="1">
+        <v>100</v>
+      </c>
+      <c r="C58" s="1">
+        <v>122</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="B58" s="1">
-        <v>0</v>
-      </c>
-      <c r="C58" s="1">
-        <v>1</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="B59" s="1">
-        <v>10</v>
       </c>
       <c r="C59" s="1">
         <v>4</v>
@@ -2487,64 +2478,64 @@
       <c r="A60" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B60" s="1">
-        <v>100</v>
+      <c r="B60" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="C60" s="1">
-        <v>122</v>
+        <v>174</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C61" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C62" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="409.5" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C63" s="1">
-        <v>176</v>
+        <v>19</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B64" s="1" t="s">
         <v>168</v>
+      </c>
+      <c r="B64" s="1">
+        <v>200</v>
       </c>
       <c r="C64" s="1">
         <v>1</v>
@@ -2561,13 +2552,13 @@
         <v>171</v>
       </c>
       <c r="C65" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>173</v>
       </c>
@@ -2575,21 +2566,21 @@
         <v>174</v>
       </c>
       <c r="C66" s="1">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>176</v>
       </c>
       <c r="B67" s="1">
-        <v>200</v>
+        <v>27</v>
       </c>
       <c r="C67" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>177</v>
@@ -2613,78 +2604,78 @@
       <c r="A69" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B69" s="1">
-        <v>27</v>
+      <c r="B69" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="C69" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C70" s="1">
         <v>1</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C71" s="1">
         <v>1</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C72" s="1">
         <v>1</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C73" s="1">
         <v>1</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B74" s="1" t="s">
         <v>196</v>
+      </c>
+      <c r="B74" s="1">
+        <v>680</v>
       </c>
       <c r="C74" s="1">
         <v>1</v>
@@ -2711,29 +2702,27 @@
       <c r="A76" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B76" s="1">
-        <v>680</v>
+      <c r="B76" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="C76" s="1">
         <v>1</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C77" s="1">
         <v>1</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>205</v>
-      </c>
+      <c r="D77" s="1"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
@@ -2745,23 +2734,23 @@
       <c r="C78" s="1">
         <v>1</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D78" s="1"/>
+    </row>
+    <row r="79" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>209</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C79" s="1">
+        <v>5</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C79" s="1">
-        <v>1</v>
-      </c>
-      <c r="D79" s="1"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="80" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>211</v>
       </c>
@@ -2769,69 +2758,71 @@
         <v>212</v>
       </c>
       <c r="C80" s="1">
-        <v>1</v>
-      </c>
-      <c r="D80" s="1"/>
-    </row>
-    <row r="81" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>214</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C81" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C82" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C83" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C84" s="1">
         <v>1</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>226</v>
@@ -2840,12 +2831,12 @@
         <v>1</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>229</v>
@@ -2854,193 +2845,165 @@
         <v>1</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>231</v>
-      </c>
       <c r="C87" s="1">
         <v>1</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>234</v>
-      </c>
       <c r="C88" s="1">
         <v>1</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="C89" s="1">
         <v>1</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="C90" s="1">
         <v>1</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>243</v>
-      </c>
       <c r="C91" s="1">
         <v>1</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B92" s="1" t="s">
-        <v>246</v>
-      </c>
       <c r="C92" s="1">
         <v>1</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>249</v>
-      </c>
       <c r="C93" s="1">
         <v>1</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B94" s="1" t="s">
-        <v>252</v>
-      </c>
       <c r="C94" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B95" s="1" t="s">
-        <v>255</v>
-      </c>
       <c r="C95" s="1">
         <v>1</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B96" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="C96" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>261</v>
-      </c>
       <c r="C97" s="1">
         <v>1</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A98" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B98" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="C98" s="1">
-        <v>8</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A99" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C99" s="1">
-        <v>1</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>269</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>